<commit_message>
Manipulated data and defined params
</commit_message>
<xml_diff>
--- a/data/distance-matrix.xlsx
+++ b/data/distance-matrix.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alqer\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACA109B-60F9-4357-814E-9DC82EA8EB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -70,9 +69,6 @@
     <t>KAYSERİ</t>
   </si>
   <si>
-    <t>KOCAELİ (İZMİT)</t>
-  </si>
-  <si>
     <t>KONYA</t>
   </si>
   <si>
@@ -94,9 +90,6 @@
     <t>RİZE</t>
   </si>
   <si>
-    <t>SAKARYA (ADAPAZARI)</t>
-  </si>
-  <si>
     <t>SAMSUN</t>
   </si>
   <si>
@@ -114,11 +107,17 @@
   <si>
     <t>CITY NAME</t>
   </si>
+  <si>
+    <t>KOCAELİ</t>
+  </si>
+  <si>
+    <t>SAKARYA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -224,7 +223,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -240,9 +239,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,9 +279,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,7 +316,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,7 +351,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -525,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -540,9 +539,9 @@
     <col min="33" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" customFormat="1" ht="102.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" customFormat="1" ht="84.75" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -593,46 +592,46 @@
         <v>15</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2125,7 +2124,7 @@
     </row>
     <row r="18" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>840</v>
@@ -2218,7 +2217,7 @@
     </row>
     <row r="19" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="10">
         <v>357</v>
@@ -2311,7 +2310,7 @@
     </row>
     <row r="20" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="10">
         <v>397</v>
@@ -2404,7 +2403,7 @@
     </row>
     <row r="21" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1">
         <v>886</v>
@@ -2497,7 +2496,7 @@
     </row>
     <row r="22" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="10">
         <v>197</v>
@@ -2590,7 +2589,7 @@
     </row>
     <row r="23" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="10">
         <v>856</v>
@@ -2683,7 +2682,7 @@
     </row>
     <row r="24" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="10">
         <v>707</v>
@@ -2776,7 +2775,7 @@
     </row>
     <row r="25" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>917</v>
@@ -2869,7 +2868,7 @@
     </row>
     <row r="26" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B26" s="10">
         <v>803</v>
@@ -2962,7 +2961,7 @@
     </row>
     <row r="27" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1">
         <v>754</v>
@@ -3055,7 +3054,7 @@
     </row>
     <row r="28" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1">
         <v>1082</v>
@@ -3148,7 +3147,7 @@
     </row>
     <row r="29" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1">
         <v>838</v>
@@ -3241,7 +3240,7 @@
     </row>
     <row r="30" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1">
         <v>355</v>
@@ -3334,7 +3333,7 @@
     </row>
     <row r="31" spans="1:31" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
         <v>900</v>

</xml_diff>

<commit_message>
Semi finalized the model
</commit_message>
<xml_diff>
--- a/data/distance-matrix.xlsx
+++ b/data/distance-matrix.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alqer\Desktop\uni\s2\supply-chain-management\project\facility-location-problem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F90241-F294-4EB0-8E21-4D955CB62238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -117,7 +118,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -223,7 +224,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1"/>
+    <cellStyle name="Normal_mesafe cetveli-2004" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,9 +240,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,9 +280,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,7 +317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,11 +525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3434,19 +3435,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="116776fd-905b-4a7f-ba2f-f1d8893a9227">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3607,27 +3601,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="116776fd-905b-4a7f-ba2f-f1d8893a9227">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58CC262A-B562-42E0-91FC-5EF403BD7CB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53CF22A-DE78-474E-9BBE-C17B89D94692}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="116776fd-905b-4a7f-ba2f-f1d8893a9227"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3652,9 +3644,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53CF22A-DE78-474E-9BBE-C17B89D94692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58CC262A-B562-42E0-91FC-5EF403BD7CB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="116776fd-905b-4a7f-ba2f-f1d8893a9227"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>